<commit_message>
base de datos tesis
</commit_message>
<xml_diff>
--- a/palabras reservadas 1.xlsx
+++ b/palabras reservadas 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigar.JUAN\Documents\GitHub\Compiladores6to\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E720A333-0E1B-49CA-A809-D49F28F32744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3FF492-580E-49D3-885F-4D0C731D50C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{68A45492-F983-419C-8157-91171356A23F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{68A45492-F983-419C-8157-91171356A23F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="241">
   <si>
     <t>se utiliza para declarar sumas</t>
   </si>
@@ -406,64 +406,6 @@
     <t>Revisa el código para eliminar las llaves que no son necesarias o que no tienen su pareja correspondiente, manteniendo la estructura del código coherente y legible.</t>
   </si>
   <si>
-    <t>Falta de pu nto y coma</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Este error ocurre cuando falta un punto y coma </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> al final de una declaración o instrucción donde es necesario según las reglas de sintaxis del lenguaje de programación.</t>
-    </r>
-  </si>
-  <si>
-    <t>Agrega un punto y coma al final de cada declaración o instrucción donde sea necesario para garantizar la correcta interpretación del código por parte del compilador o intérprete.</t>
-  </si>
-  <si>
-    <t>Sobran puntos y comas</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Este error ocurre cuando hay puntos y coma </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> adicionales al final de las declaraciones que no son necesarios según las reglas de sintaxis del lenguaje de programación.</t>
-    </r>
-  </si>
-  <si>
-    <t>Elimina los puntos y coma adicionales al final de las declaraciones para mantener el código limpio y evitar posibles errores de interpretación</t>
-  </si>
-  <si>
     <t xml:space="preserve">Errores de indentacion </t>
   </si>
   <si>
@@ -910,6 +852,63 @@
   </si>
   <si>
     <t>se usa para declarar variables de fecha</t>
+  </si>
+  <si>
+    <t>Tristana</t>
+  </si>
+  <si>
+    <t>En un bucle,  se utiliza para salir del bucle antes de que se complete la iteración normal</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Talon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> se utiliza  para devolver un valor de una función</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Falta de OR (|)</t>
+  </si>
+  <si>
+    <t>Este error ocurre cuando falta un OR | al final de una declaración o instrucción donde es necesario según las reglas de sintaxis del lenguaje de programación.</t>
+  </si>
+  <si>
+    <t>Agrega (OR) | al final de cada declaración o instrucción donde sea necesario para garantizar la correcta interpretación del código por parte del compilador o intérprete.</t>
+  </si>
+  <si>
+    <t>Sobran (OR) |</t>
+  </si>
+  <si>
+    <t>Este error ocurre cuando hay (OR) | adicionales al final de las declaraciones que no son necesarios según las reglas de sintaxis del lenguaje de programación.</t>
+  </si>
+  <si>
+    <t>Elimina (OR) | adicionales al final de las declaraciones para mantener el código limpio y evitar posibles errores de interpretación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta cerrar parentecis </t>
+  </si>
+  <si>
+    <t>Faltan cerrar los parentecis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pon el parentecis faltante para corregir el error </t>
+  </si>
+  <si>
+    <t>Falta retornar a la variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anexa la palabra return para retornar la variable y  corregir el error </t>
+  </si>
+  <si>
+    <t>Falta de return</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1213,6 +1212,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1528,25 +1530,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46073DD4-5167-4E75-9515-EDCF81F3CCF4}">
-  <dimension ref="B1:L62"/>
+  <dimension ref="B1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="3" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="25" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="25" customWidth="1"/>
+    <col min="6" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="21.140625" style="7" customWidth="1"/>
+    <col min="9" max="11" width="21.109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="22" t="s">
         <v>12</v>
@@ -1568,7 +1570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1594,7 +1596,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -1621,7 +1623,7 @@
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1647,7 +1649,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1673,7 +1675,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:12" s="1" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" s="1" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>5</v>
       </c>
@@ -1681,7 +1683,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>62</v>
@@ -1701,7 +1703,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:12" s="1" customFormat="1" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" s="1" customFormat="1" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>63</v>
@@ -1729,7 +1731,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="135" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1737,7 +1739,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>64</v>
@@ -1755,7 +1757,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="105" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -1763,7 +1765,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>65</v>
@@ -1781,7 +1783,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="120" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -1789,7 +1791,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>66</v>
@@ -1807,7 +1809,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="120" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>10</v>
       </c>
@@ -1815,7 +1817,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>67</v>
@@ -1833,7 +1835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="96.6" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>68</v>
@@ -1859,7 +1861,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="120" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -1867,7 +1869,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>69</v>
@@ -1885,7 +1887,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="135" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -1893,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>70</v>
@@ -1902,16 +1904,16 @@
         <v>13</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>98</v>
+        <v>228</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>99</v>
+        <v>229</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="114" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="105" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>14</v>
       </c>
@@ -1919,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E16" s="27" t="s">
         <v>71</v>
@@ -1928,16 +1930,16 @@
         <v>14</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>101</v>
+        <v>231</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>102</v>
+        <v>232</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="128.25" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="135" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>15</v>
       </c>
@@ -1945,7 +1947,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E17" s="27" t="s">
         <v>72</v>
@@ -1954,24 +1956,24 @@
         <v>15</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="142.5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="150" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>16</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E18" s="27" t="s">
         <v>73</v>
@@ -1980,16 +1982,16 @@
         <v>16</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="128.25" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="135" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>17</v>
       </c>
@@ -1997,7 +1999,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>74</v>
@@ -2006,16 +2008,16 @@
         <v>17</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="71.25" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="75" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>18</v>
       </c>
@@ -2023,7 +2025,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>75</v>
@@ -2032,16 +2034,16 @@
         <v>18</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="85.5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="90" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>19</v>
       </c>
@@ -2049,7 +2051,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E21" s="27" t="s">
         <v>76</v>
@@ -2058,16 +2060,16 @@
         <v>19</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="99.75" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="105" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>20</v>
       </c>
@@ -2075,7 +2077,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E22" s="27" t="s">
         <v>77</v>
@@ -2084,16 +2086,16 @@
         <v>20</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="128.25" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="150" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>21</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E23" s="27" t="s">
         <v>78</v>
@@ -2110,16 +2112,16 @@
         <v>21</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="63.75" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="69" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>22</v>
       </c>
@@ -2127,7 +2129,7 @@
         <v>11</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E24" s="27" t="s">
         <v>79</v>
@@ -2136,16 +2138,16 @@
         <v>22</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="K24" s="36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>23</v>
       </c>
@@ -2159,27 +2161,27 @@
         <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H25" s="21">
         <v>23</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>24</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>88</v>
@@ -2187,503 +2189,558 @@
       <c r="E26" s="27" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="H26" s="10">
+        <v>24</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>25</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="H27" s="10">
+        <v>25</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>26</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>27</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
         <v>28</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B31" s="5">
         <v>29</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>30</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="5">
         <v>31</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B34" s="5">
         <v>32</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B35" s="5">
         <v>33</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B36" s="5">
         <v>34</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B37" s="6">
         <v>35</v>
       </c>
-      <c r="C37" s="24" t="s">
-        <v>90</v>
+      <c r="C37" s="38" t="s">
+        <v>222</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B38" s="5">
         <v>36</v>
       </c>
-      <c r="C38" s="27" t="s">
-        <v>143</v>
+      <c r="C38" s="38" t="s">
+        <v>225</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="27"/>
-    </row>
-    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5">
         <v>37</v>
       </c>
-      <c r="C39" s="27"/>
+      <c r="C39" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="D39" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="27"/>
-    </row>
-    <row r="40" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B40" s="5">
         <v>38</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E40" s="27" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="E40" s="27"/>
+    </row>
+    <row r="41" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B41" s="5">
         <v>39</v>
       </c>
-      <c r="C41" s="27" t="s">
-        <v>148</v>
-      </c>
+      <c r="C41" s="27"/>
       <c r="D41" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="27" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="E41" s="27"/>
+    </row>
+    <row r="42" spans="2:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B42" s="6">
         <v>40</v>
       </c>
-      <c r="C42" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B43" s="5">
         <v>41</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5">
         <v>42</v>
       </c>
-      <c r="C44" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C44" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="5">
         <v>43</v>
       </c>
-      <c r="C45" s="32" t="s">
-        <v>154</v>
+      <c r="C45" s="27" t="s">
+        <v>144</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B46" s="5">
         <v>44</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B47" s="6">
         <v>45</v>
       </c>
-      <c r="C47" s="27" t="s">
-        <v>158</v>
+      <c r="C47" s="32" t="s">
+        <v>148</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" s="27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B48" s="5">
         <v>46</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="5">
         <v>47</v>
       </c>
-      <c r="C49" s="33" t="s">
-        <v>163</v>
+      <c r="C49" s="27" t="s">
+        <v>152</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="5">
         <v>48</v>
       </c>
-      <c r="C50" s="31" t="s">
-        <v>165</v>
+      <c r="C50" s="27" t="s">
+        <v>154</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B51" s="5">
         <v>49</v>
       </c>
-      <c r="C51" s="27" t="s">
-        <v>173</v>
+      <c r="C51" s="33" t="s">
+        <v>157</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="6">
         <v>50</v>
       </c>
-      <c r="C52" s="32" t="s">
-        <v>175</v>
+      <c r="C52" s="31" t="s">
+        <v>159</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="27" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B53" s="5">
         <v>51</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B54" s="5">
         <v>52</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B55" s="5">
         <v>53</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="5">
         <v>54</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57" s="6">
         <v>55</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="5">
         <v>56</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B59" s="5">
         <v>57</v>
       </c>
-      <c r="C59" s="32" t="s">
-        <v>187</v>
+      <c r="C59" s="27" t="s">
+        <v>177</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B60" s="5">
         <v>58</v>
       </c>
-      <c r="C60" s="15" t="s">
-        <v>197</v>
+      <c r="C60" s="32" t="s">
+        <v>179</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B61" s="5">
+        <v>59</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B62" s="6">
+        <v>60</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B63" s="5">
+        <v>61</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B64" s="5">
+        <v>62</v>
+      </c>
+      <c r="C64" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="E60" s="27" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B61" s="6">
-        <v>59</v>
-      </c>
-      <c r="C61" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" s="35" t="s">
+      <c r="D64" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E61" s="29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B62" s="5">
-        <v>60</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E62" s="27" t="s">
-        <v>205</v>
+      <c r="E64" s="27" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update palabras reservadas 1.xlsx
</commit_message>
<xml_diff>
--- a/palabras reservadas 1.xlsx
+++ b/palabras reservadas 1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigar.JUAN\Documents\GitHub\Compiladores6to\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3FF492-580E-49D3-885F-4D0C731D50C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{68A45492-F983-419C-8157-91171356A23F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="240">
   <si>
     <t>se utiliza para declarar sumas</t>
   </si>
@@ -907,14 +906,11 @@
   <si>
     <t>Falta de return</t>
   </si>
-  <si>
-    <t>o</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1529,11 +1525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46073DD4-5167-4E75-9515-EDCF81F3CCF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2241,9 +2237,6 @@
       <c r="E28" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="29" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="5">

</xml_diff>

<commit_message>
no puedo marta :(
AAAAAAYYYYYYYUUUUUUUUDDDDDDDAAAAAAAA!!!!!!!
</commit_message>
<xml_diff>
--- a/palabras reservadas 1.xlsx
+++ b/palabras reservadas 1.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="274">
   <si>
     <t>|</t>
   </si>
@@ -1208,6 +1208,15 @@
   </si>
   <si>
     <t>Letra</t>
+  </si>
+  <si>
+    <t>Fiora</t>
+  </si>
+  <si>
+    <t>se utiliza para imprimir en la consola junto con write y writeline</t>
+  </si>
+  <si>
+    <t>Console</t>
   </si>
 </sst>
 </file>
@@ -1898,10 +1907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L81"/>
+  <dimension ref="B1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3330,6 +3339,20 @@
       </c>
       <c r="E81" s="25"/>
     </row>
+    <row r="82" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B82" s="43">
+        <v>80</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="E82" s="25" t="s">
+        <v>273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>